<commit_message>
draft2 with 50 videos per youtube channel
</commit_message>
<xml_diff>
--- a/YouTubeFacebookVideo/draft1.xlsx
+++ b/YouTubeFacebookVideo/draft1.xlsx
@@ -677,7 +677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>